<commit_message>
Update execution counts in Jupyter notebook and modify Excel writer to use 'openpyxl' engine. Adjust figure sizes in outputs and update Python version in metadata. Also, refresh the 'R&D_2025_Combined_Frequency_Tables.xlsx' file.
</commit_message>
<xml_diff>
--- a/R&D_2025_Combined_Frequency_Tables.xlsx
+++ b/R&D_2025_Combined_Frequency_Tables.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="All_Frequencies" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Frequency_Tables" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Awareness_Perception_Frequencies" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Scores_Statistics" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Score_Categories" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Score_Percentages" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="All_Frequencies" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Frequency_Tables" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Awareness_Perception_Frequencies" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Scores_Statistics" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Score_Categories" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Score_Percentages" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Scores_Correlation" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -22,10 +22,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -42,12 +50,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -60,14 +83,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -432,7 +458,7 @@
   </sheetPr>
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -940,7 +966,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -993,7 +1019,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1012,22 +1038,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Column</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Correct</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Wrong</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -1181,32 +1207,32 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Original_Column</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Strongly agree</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Agree</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Not sure</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Disagree</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Strongly disagree</t>
         </is>
@@ -1606,19 +1632,19 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Mean</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Standard Deviation</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>knowledge_score</t>
         </is>
@@ -1631,7 +1657,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>awareness_Score</t>
         </is>
@@ -1644,7 +1670,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>perception_Score</t>
         </is>
@@ -1676,24 +1702,24 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Knowledge</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Awareness</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Perception</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Good</t>
         </is>
@@ -1709,7 +1735,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Poor</t>
         </is>
@@ -1744,24 +1770,24 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Knowledge</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Awareness</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Perception</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Good</t>
         </is>
@@ -1777,7 +1803,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Poor</t>
         </is>
@@ -1790,6 +1816,127 @@
       </c>
       <c r="D3" t="n">
         <v>93.21266968325791</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Variable</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Variable</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>knowledge_score</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>awareness_Score</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>perception_Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>knowledge_score</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1.000 (p=0.000)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>0.321 (p=0.000)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0.219 (p=0.001)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>awareness_Score</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.321 (p=0.000)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1.000 (p=0.000)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0.239 (p=0.000)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>perception_Score</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.219 (p=0.001)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0.239 (p=0.000)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1.000 (p=0.000)</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>